<commit_message>
Slight update on generic benchmark Excel
</commit_message>
<xml_diff>
--- a/tensorflow_MNIST/results/generic_benchmark.xlsx
+++ b/tensorflow_MNIST/results/generic_benchmark.xlsx
@@ -289,7 +289,6 @@
                   <a:rPr lang="en-US"/>
                   <a:t>data size (kB)</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -407,7 +406,6 @@
                   <a:rPr lang="en-US"/>
                   <a:t>Speedup ratio</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -2101,16 +2099,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>251460</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>556260</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2138,15 +2136,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>365760</xdr:colOff>
+      <xdr:colOff>335280</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>83820</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2474,7 +2472,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+      <selection activeCell="S10" sqref="S10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>